<commit_message>
edit the raw data
</commit_message>
<xml_diff>
--- a/raw_data/location.xlsx
+++ b/raw_data/location.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gayoungp/Desktop/KoreaNeolithicfishingtools/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366072E5-F5A6-5748-99B6-85317BAD3CB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DABD93-15C7-CD48-A34B-1A18EA21293D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="460" windowWidth="20900" windowHeight="15540" xr2:uid="{636B16D6-7A8C-4EE6-A103-70930B4A2A10}"/>
+    <workbookView xWindow="17080" yWindow="460" windowWidth="20900" windowHeight="15540" xr2:uid="{636B16D6-7A8C-4EE6-A103-70930B4A2A10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2311,7 +2311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45AD748-62BD-45B7-9619-88D9BF1D586F}">
   <dimension ref="A1:M191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F138" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>

</xml_diff>